<commit_message>
ucs2 - coding8 added, openpyxl
</commit_message>
<xml_diff>
--- a/small_test.xlsx
+++ b/small_test.xlsx
@@ -47,10 +47,10 @@
     <t>Vitajte v našej skutočnej aplikácii!</t>
   </si>
   <si>
-    <t>Vaša VšZP</t>
-  </si>
-  <si>
     <t>420987123452</t>
+  </si>
+  <si>
+    <t>TESTING</t>
   </si>
 </sst>
 </file>
@@ -375,7 +375,7 @@
   <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -385,7 +385,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
@@ -400,7 +400,7 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
test diplicity, updated coding=4
</commit_message>
<xml_diff>
--- a/small_test.xlsx
+++ b/small_test.xlsx
@@ -372,10 +372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A12"/>
+  <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A3" sqref="A3:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -423,10 +423,19 @@
         <v>4</v>
       </c>
     </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+    </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>